<commit_message>
Added most of the BibTeX information for the fluids - 90% done
</commit_message>
<xml_diff>
--- a/Vault/Lennard Jones coefficients from The Properties of Gases and Liquids.xlsx
+++ b/Vault/Lennard Jones coefficients from The Properties of Gases and Liquids.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>Argon</t>
   </si>
@@ -628,33 +628,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -664,8 +665,17 @@
       <c r="C6" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -675,8 +685,17 @@
       <c r="C7">
         <v>93.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>4.7610000000000001</v>
+      </c>
+      <c r="H7">
+        <v>251.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -686,8 +705,17 @@
       <c r="C8">
         <v>10.220000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8">
+        <v>4.8070000000000004</v>
+      </c>
+      <c r="H8">
+        <v>248.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -697,8 +725,17 @@
       <c r="C9">
         <v>178.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9">
+        <v>5.1180000000000003</v>
+      </c>
+      <c r="H9">
+        <v>237.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -708,8 +745,17 @@
       <c r="C10">
         <v>32.799999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10">
+        <v>4.5490000000000004</v>
+      </c>
+      <c r="H10">
+        <v>576.70000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -719,8 +765,17 @@
       <c r="C11">
         <v>231</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H11">
+        <v>560.20000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -730,8 +785,17 @@
       <c r="C12">
         <v>78.599999999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <v>4.9359999999999999</v>
+      </c>
+      <c r="H12">
+        <v>469.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -741,8 +805,17 @@
       <c r="C13">
         <v>259.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13">
+        <v>4.6870000000000003</v>
+      </c>
+      <c r="H13">
+        <v>531.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -752,8 +825,17 @@
       <c r="C14">
         <v>337.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14">
+        <v>5.2779999999999996</v>
+      </c>
+      <c r="H14">
+        <v>330.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -763,8 +845,17 @@
       <c r="C15">
         <v>186.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H15">
+        <v>313.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -774,8 +865,17 @@
       <c r="C16">
         <v>396.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16">
+        <v>5.2050000000000001</v>
+      </c>
+      <c r="H16">
+        <v>521.29999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -785,8 +885,17 @@
       <c r="C17">
         <v>507.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17">
+        <v>5.7839999999999998</v>
+      </c>
+      <c r="H17">
+        <v>341.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -796,8 +905,17 @@
       <c r="C18">
         <v>322.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18">
+        <v>6.4640000000000004</v>
+      </c>
+      <c r="H18">
+        <v>193.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -807,8 +925,17 @@
       <c r="C19">
         <v>134</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19">
+        <v>5.3490000000000002</v>
+      </c>
+      <c r="H19">
+        <v>412.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -818,8 +945,17 @@
       <c r="C20">
         <v>340.2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20">
+        <v>6.1820000000000004</v>
+      </c>
+      <c r="H20">
+        <v>297.10000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -829,8 +965,17 @@
       <c r="C21">
         <v>356.3</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21">
+        <v>5.9489999999999998</v>
+      </c>
+      <c r="H21">
+        <v>399.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -840,8 +985,17 @@
       <c r="C22">
         <v>449.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G22">
+        <v>4.2169999999999996</v>
+      </c>
+      <c r="H22">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -851,8 +1005,17 @@
       <c r="C23">
         <v>350</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23">
+        <v>3.3570000000000002</v>
+      </c>
+      <c r="H23">
+        <v>112.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -862,8 +1025,17 @@
       <c r="C24">
         <v>481.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24">
+        <v>3.3530000000000002</v>
+      </c>
+      <c r="H24">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -873,8 +1045,17 @@
       <c r="C25">
         <v>148.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25">
+        <v>3.63</v>
+      </c>
+      <c r="H25">
+        <v>569.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -884,8 +1065,17 @@
       <c r="C26">
         <v>91.7</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26">
+        <v>3.339</v>
+      </c>
+      <c r="H26">
+        <v>344.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -895,8 +1085,17 @@
       <c r="C27">
         <v>336</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+      <c r="G27">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="H27">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -906,8 +1105,17 @@
       <c r="C28">
         <v>195.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>51</v>
+      </c>
+      <c r="G28">
+        <v>4.2110000000000003</v>
+      </c>
+      <c r="H28">
+        <v>288.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -917,8 +1125,17 @@
       <c r="C29">
         <v>467</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29">
+        <v>2.827</v>
+      </c>
+      <c r="H29">
+        <v>59.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -928,8 +1145,17 @@
       <c r="C30">
         <v>231.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G30">
+        <v>2.641</v>
+      </c>
+      <c r="H30">
+        <v>809.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -939,8 +1165,17 @@
       <c r="C31">
         <v>224.7</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31">
+        <v>4.1959999999999997</v>
+      </c>
+      <c r="H31">
+        <v>289.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -950,8 +1185,17 @@
       <c r="C32">
         <v>215.7</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G32">
+        <v>3.6230000000000002</v>
+      </c>
+      <c r="H32">
+        <v>301.10000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -961,8 +1205,17 @@
       <c r="C33">
         <v>300</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33">
+        <v>2.9689999999999999</v>
+      </c>
+      <c r="H33">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -972,8 +1225,17 @@
       <c r="C34">
         <v>362.6</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34">
+        <v>5.08</v>
+      </c>
+      <c r="H34">
+        <v>686.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -983,8 +1245,17 @@
       <c r="C35">
         <v>348.6</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35">
+        <v>4.55</v>
+      </c>
+      <c r="H35">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -994,8 +1265,17 @@
       <c r="C36">
         <v>395</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>59</v>
+      </c>
+      <c r="G36">
+        <v>5.625</v>
+      </c>
+      <c r="H36">
+        <v>695.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1005,488 +1285,156 @@
       <c r="C37">
         <v>298.89999999999998</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39">
-        <v>4.7610000000000001</v>
-      </c>
-      <c r="C39">
-        <v>251.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40">
-        <v>4.8070000000000004</v>
-      </c>
-      <c r="C40">
-        <v>248.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41">
-        <v>5.1180000000000003</v>
-      </c>
-      <c r="C41">
-        <v>237.1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42">
-        <v>4.5490000000000004</v>
-      </c>
-      <c r="C42">
-        <v>576.70000000000005</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="C43">
-        <v>560.20000000000005</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B44">
-        <v>4.9359999999999999</v>
-      </c>
-      <c r="C44">
-        <v>469.8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45">
-        <v>4.6870000000000003</v>
-      </c>
-      <c r="C45">
-        <v>531.4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46">
-        <v>5.2779999999999996</v>
-      </c>
-      <c r="C46">
-        <v>330.1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="C47">
-        <v>313.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48">
-        <v>5.2050000000000001</v>
-      </c>
-      <c r="C48">
-        <v>521.29999999999995</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>40</v>
-      </c>
-      <c r="B49">
-        <v>5.7839999999999998</v>
-      </c>
-      <c r="C49">
-        <v>341.1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B50">
-        <v>6.4640000000000004</v>
-      </c>
-      <c r="C50">
-        <v>193.4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>42</v>
-      </c>
-      <c r="B51">
-        <v>5.3490000000000002</v>
-      </c>
-      <c r="C51">
-        <v>412.3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>43</v>
-      </c>
-      <c r="B52">
-        <v>6.1820000000000004</v>
-      </c>
-      <c r="C52">
-        <v>297.10000000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>44</v>
-      </c>
-      <c r="B53">
-        <v>5.9489999999999998</v>
-      </c>
-      <c r="C53">
-        <v>399.3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>45</v>
-      </c>
-      <c r="B54">
-        <v>4.2169999999999996</v>
-      </c>
-      <c r="C54">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>46</v>
-      </c>
-      <c r="B55">
-        <v>3.3570000000000002</v>
-      </c>
-      <c r="C55">
-        <v>112.6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>47</v>
-      </c>
-      <c r="B56">
-        <v>3.3530000000000002</v>
-      </c>
-      <c r="C56">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>48</v>
-      </c>
-      <c r="B57">
-        <v>3.63</v>
-      </c>
-      <c r="C57">
-        <v>569.1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>49</v>
-      </c>
-      <c r="B58">
-        <v>3.339</v>
-      </c>
-      <c r="C58">
-        <v>344.7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>50</v>
-      </c>
-      <c r="B59">
-        <v>3.1480000000000001</v>
-      </c>
-      <c r="C59">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>51</v>
-      </c>
-      <c r="B60">
-        <v>4.2110000000000003</v>
-      </c>
-      <c r="C60">
-        <v>288.7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>52</v>
-      </c>
-      <c r="B61">
-        <v>2.827</v>
-      </c>
-      <c r="C61">
-        <v>59.7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>53</v>
-      </c>
-      <c r="B62">
-        <v>2.641</v>
-      </c>
-      <c r="C62">
-        <v>809.1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B63">
-        <v>4.1959999999999997</v>
-      </c>
-      <c r="C63">
-        <v>289.3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>55</v>
-      </c>
-      <c r="B64">
-        <v>3.6230000000000002</v>
-      </c>
-      <c r="C64">
-        <v>301.10000000000002</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>56</v>
-      </c>
-      <c r="B65">
-        <v>2.9689999999999999</v>
-      </c>
-      <c r="C65">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>57</v>
-      </c>
-      <c r="B66">
-        <v>5.08</v>
-      </c>
-      <c r="C66">
-        <v>686.2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>58</v>
-      </c>
-      <c r="B67">
-        <v>4.55</v>
-      </c>
-      <c r="C67">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>59</v>
-      </c>
-      <c r="B68">
-        <v>5.625</v>
-      </c>
-      <c r="C68">
-        <v>695.6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="F37" t="s">
         <v>60</v>
       </c>
-      <c r="B69">
+      <c r="G37">
         <v>5.16</v>
       </c>
-      <c r="C69">
+      <c r="H37">
         <v>474.2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
         <v>61</v>
       </c>
-      <c r="B70">
+      <c r="G38">
         <v>2.9</v>
       </c>
-      <c r="C70">
+      <c r="H38">
         <v>558.29999999999995</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
         <v>62</v>
       </c>
-      <c r="B71">
+      <c r="G39">
         <v>3.492</v>
       </c>
-      <c r="C71">
+      <c r="H39">
         <v>116.7</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
         <v>63</v>
       </c>
-      <c r="B72">
+      <c r="G40">
         <v>4.1120000000000001</v>
       </c>
-      <c r="C72">
+      <c r="H40">
         <v>395.3</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
         <v>64</v>
       </c>
-      <c r="B73">
+      <c r="G41">
         <v>3.798</v>
       </c>
-      <c r="C73">
+      <c r="H41">
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
         <v>65</v>
       </c>
-      <c r="B74">
+      <c r="G42">
         <v>3.8279999999999998</v>
       </c>
-      <c r="C74">
+      <c r="H42">
         <v>232.4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
         <v>66</v>
       </c>
-      <c r="B75">
+      <c r="G43">
         <v>3.4670000000000001</v>
       </c>
-      <c r="C75">
+      <c r="H43">
         <v>106.7</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
         <v>67</v>
       </c>
-      <c r="B76">
+      <c r="G44">
         <v>3.9809999999999999</v>
       </c>
-      <c r="C76">
+      <c r="H44">
         <v>251.5</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
         <v>74</v>
       </c>
-      <c r="B77">
+      <c r="G45">
         <v>5.1280000000000001</v>
       </c>
-      <c r="C77">
+      <c r="H45">
         <v>222.1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
         <v>68</v>
       </c>
-      <c r="B78">
+      <c r="G46">
         <v>4.1120000000000001</v>
       </c>
-      <c r="C78">
+      <c r="H46">
         <v>335.4</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
         <v>69</v>
       </c>
-      <c r="B79">
+      <c r="G47">
         <v>4.88</v>
       </c>
-      <c r="C79">
+      <c r="H47">
         <v>171.9</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
         <v>70</v>
       </c>
-      <c r="B80">
+      <c r="G48">
         <v>4.0839999999999996</v>
       </c>
-      <c r="C80">
+      <c r="H48">
         <v>207.6</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="49" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
         <v>71</v>
       </c>
-      <c r="B81">
+      <c r="G49">
         <v>6.3879999999999999</v>
       </c>
-      <c r="C81">
+      <c r="H49">
         <v>563.70000000000005</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="50" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
         <v>72</v>
       </c>
-      <c r="B82">
+      <c r="G50">
         <v>5.9669999999999996</v>
       </c>
-      <c r="C82">
+      <c r="H50">
         <v>236.8</v>
       </c>
     </row>

</xml_diff>